<commit_message>
edited the method template
git-svn-id: https://forge.cornell.edu/svn/repos/automated_design@5023 d22a8b0d-b447-0410-a14f-ca4c0a428a39

Former-commit-id: 5e1578f0cfd3a2c18d7765ab2739605ce787a7b2
</commit_message>
<xml_diff>
--- a/Final Designs/ADT Designs/Method template.xlsx
+++ b/Final Designs/ADT Designs/Method template.xlsx
@@ -1,23 +1,246 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="28620" windowHeight="12915"/>
+    <workbookView xWindow="12600" yWindow="-15" windowWidth="12645" windowHeight="12345"/>
   </bookViews>
   <sheets>
     <sheet name="Method" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>her28</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>her28:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Do not change what is in the red boxes, ever. Change the other inputs to fit the method you are working on and insert rows for more user inputs as necessary.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>her28:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+"rank" essential means how high do you want this design on the designs webpage? The plant, EtFlocSedFi, should be 1.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>her28:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+include as many stock designs as you feel is appropriate for your specific method, make you fill in all necessary variables for all designs you want</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>her28:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+make sure this is the actual variable name used in the associated mathcad code</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>her28:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+min, max, default and increment limit the user into entering appropriate values when requesting a design</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>her28:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+starting from this column, this row states the titles of each stock design you create</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>her28:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+the first user input should almost always be the plant flow rate, Q.Plant</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>her28:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+you can have as many user inputs listed here as is necessary for this specific method</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>her28:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+this is the AC variable that is left undefined at the bottom of the mathcad file associated with this method, if you have multiple output variables, list them in this row</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
-  <si>
-    <t>The LFOM method creates a linear flow orifice meter based on the target range of head and flow rate.</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>Input parameters</t>
   </si>
@@ -97,21 +320,9 @@
     <t>150Lps</t>
   </si>
   <si>
-    <t>Maximum flow for the flow meter</t>
-  </si>
-  <si>
-    <t>Q.Plant</t>
-  </si>
-  <si>
     <t>L/s</t>
   </si>
   <si>
-    <t>Height range for the flow meter</t>
-  </si>
-  <si>
-    <t>HL.Lfom</t>
-  </si>
-  <si>
     <t>cm</t>
   </si>
   <si>
@@ -124,20 +335,47 @@
     <t>AC variables</t>
   </si>
   <si>
-    <t>LFOM</t>
-  </si>
-  <si>
-    <t>AC.LFOM</t>
-  </si>
-  <si>
     <t>Method Rank in web page</t>
+  </si>
+  <si>
+    <t>Description of what is being created and what user inputs it is based on.</t>
+  </si>
+  <si>
+    <t>User Input 1</t>
+  </si>
+  <si>
+    <t>User Input 2</t>
+  </si>
+  <si>
+    <t>variable name 1 (Q.Plant)</t>
+  </si>
+  <si>
+    <t>variable name 2</t>
+  </si>
+  <si>
+    <t>User Input…</t>
+  </si>
+  <si>
+    <t>variable name…</t>
+  </si>
+  <si>
+    <t>filename of method</t>
+  </si>
+  <si>
+    <t>output AC.method variable</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>output AC.method variable 2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -273,8 +511,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -452,6 +710,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -615,9 +879,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -748,7 +1014,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -783,7 +1048,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -959,117 +1223,123 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:X9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="18.5703125" customWidth="1"/>
+    <col min="2" max="2" width="23.85546875" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" customWidth="1"/>
+    <col min="7" max="7" width="13" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>38</v>
+        <v>32</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="C1">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:24">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="1" t="s">
+    </row>
+    <row r="3" spans="1:24">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="B3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3" t="s">
+        <v>12</v>
+      </c>
+      <c r="L3" t="s">
+        <v>13</v>
+      </c>
+      <c r="M3" t="s">
+        <v>14</v>
+      </c>
+      <c r="N3" t="s">
+        <v>15</v>
+      </c>
+      <c r="O3" t="s">
+        <v>16</v>
+      </c>
+      <c r="P3" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>18</v>
+      </c>
+      <c r="R3" t="s">
+        <v>19</v>
+      </c>
+      <c r="S3" t="s">
+        <v>20</v>
+      </c>
+      <c r="T3" t="s">
+        <v>21</v>
+      </c>
+      <c r="U3" t="s">
+        <v>22</v>
+      </c>
+      <c r="V3" t="s">
+        <v>23</v>
+      </c>
+      <c r="W3" t="s">
+        <v>24</v>
+      </c>
+      <c r="X3" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I3" t="s">
-        <v>11</v>
-      </c>
-      <c r="J3" t="s">
-        <v>12</v>
-      </c>
-      <c r="K3" t="s">
-        <v>13</v>
-      </c>
-      <c r="L3" t="s">
-        <v>14</v>
-      </c>
-      <c r="M3" t="s">
-        <v>15</v>
-      </c>
-      <c r="N3" t="s">
-        <v>16</v>
-      </c>
-      <c r="O3" t="s">
-        <v>17</v>
-      </c>
-      <c r="P3" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>19</v>
-      </c>
-      <c r="R3" t="s">
-        <v>20</v>
-      </c>
-      <c r="S3" t="s">
-        <v>21</v>
-      </c>
-      <c r="T3" t="s">
-        <v>22</v>
-      </c>
-      <c r="U3" t="s">
-        <v>23</v>
-      </c>
-      <c r="V3" t="s">
-        <v>24</v>
-      </c>
-      <c r="W3" t="s">
-        <v>25</v>
-      </c>
-      <c r="X3" t="s">
+    <row r="4" spans="1:24">
+      <c r="A4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" t="s">
-        <v>29</v>
       </c>
       <c r="D4">
         <v>0.1</v>
@@ -1135,15 +1405,15 @@
         <v>150</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="C5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D5">
         <v>10</v>
@@ -1209,30 +1479,108 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" s="1"/>
+    <row r="6" spans="1:24">
+      <c r="A6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>100</v>
+      </c>
+      <c r="F6">
+        <v>50</v>
+      </c>
+      <c r="G6">
+        <v>0.5</v>
+      </c>
+      <c r="H6">
+        <v>50</v>
+      </c>
+      <c r="I6">
+        <v>50</v>
+      </c>
+      <c r="J6">
+        <v>50</v>
+      </c>
+      <c r="K6">
+        <v>50</v>
+      </c>
+      <c r="L6">
+        <v>50</v>
+      </c>
+      <c r="M6">
+        <v>50</v>
+      </c>
+      <c r="N6">
+        <v>50</v>
+      </c>
+      <c r="O6">
+        <v>50</v>
+      </c>
+      <c r="P6">
+        <v>50</v>
+      </c>
+      <c r="Q6">
+        <v>50</v>
+      </c>
+      <c r="R6">
+        <v>50</v>
+      </c>
+      <c r="S6">
+        <v>50</v>
+      </c>
+      <c r="T6">
+        <v>50</v>
+      </c>
+      <c r="U6" s="3">
+        <v>50</v>
+      </c>
+      <c r="V6">
+        <v>50</v>
+      </c>
+      <c r="W6">
+        <v>50</v>
+      </c>
+      <c r="X6">
+        <v>50</v>
+      </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>35</v>
-      </c>
+    <row r="7" spans="1:24">
+      <c r="A7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="1"/>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>36</v>
-      </c>
-      <c r="B8" t="s">
-        <v>37</v>
+    <row r="8" spans="1:24">
+      <c r="A8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:24">
+      <c r="A9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added field for AI.Preview
git-svn-id: https://forge.cornell.edu/svn/repos/automated_design@5065 d22a8b0d-b447-0410-a14f-ca4c0a428a39

Former-commit-id: 31f534f6905b0f97ea21ba8dcfd5fba84b1d514a
</commit_message>
<xml_diff>
--- a/Final Designs/ADT Designs/Method template.xlsx
+++ b/Final Designs/ADT Designs/Method template.xlsx
@@ -235,12 +235,36 @@
         </r>
       </text>
     </comment>
+    <comment ref="E9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>her28:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+this should always follow the last AC.method that you have</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>Input parameters</t>
   </si>
@@ -375,6 +399,12 @@
   </si>
   <si>
     <t>AguaClara Plant</t>
+  </si>
+  <si>
+    <t>output AC.method variable last</t>
+  </si>
+  <si>
+    <t>AI.Preview</t>
   </si>
 </sst>
 </file>
@@ -1234,15 +1264,16 @@
   <dimension ref="A1:X9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.5703125" customWidth="1"/>
     <col min="2" max="2" width="23.85546875" customWidth="1"/>
-    <col min="3" max="3" width="19.85546875" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="27" customWidth="1"/>
+    <col min="4" max="4" width="29.28515625" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" customWidth="1"/>
     <col min="7" max="7" width="13" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1590,6 +1621,12 @@
       </c>
       <c r="C9" t="s">
         <v>42</v>
+      </c>
+      <c r="D9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>